<commit_message>
Export phone availability for Kenya and Senegal
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict_kenya.xlsx
+++ b/inst/extdata/main_dict_kenya.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="612">
   <si>
     <t>old</t>
   </si>
@@ -1851,6 +1851,15 @@
   </si>
   <si>
     <t>yg_infant_ctg</t>
+  </si>
+  <si>
+    <t>crfs-t02b-a4_a_10a</t>
+  </si>
+  <si>
+    <t>phone_nb_avail</t>
+  </si>
+  <si>
+    <t>a4_a_10a</t>
   </si>
 </sst>
 </file>
@@ -2271,10 +2280,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H207"/>
+  <dimension ref="A1:H208"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3563,11 +3572,11 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="9" t="s">
-        <v>372</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>38</v>
+      <c r="A50" s="11" t="s">
+        <v>609</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>610</v>
       </c>
       <c r="C50" s="2">
         <v>0</v>
@@ -3576,24 +3585,24 @@
         <v>1</v>
       </c>
       <c r="E50" s="4">
-        <v>0</v>
-      </c>
-      <c r="F50" s="4">
+        <v>1</v>
+      </c>
+      <c r="F50" s="3">
         <v>0</v>
       </c>
       <c r="G50" s="3">
-        <v>0</v>
-      </c>
-      <c r="H50" s="9" t="s">
-        <v>209</v>
+        <v>1</v>
+      </c>
+      <c r="H50" s="11" t="s">
+        <v>611</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C51" s="2">
         <v>0</v>
@@ -3611,15 +3620,15 @@
         <v>0</v>
       </c>
       <c r="H51" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
-        <v>487</v>
+        <v>373</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>491</v>
+        <v>39</v>
       </c>
       <c r="C52" s="2">
         <v>0</v>
@@ -3637,15 +3646,15 @@
         <v>0</v>
       </c>
       <c r="H52" s="9" t="s">
-        <v>489</v>
+        <v>210</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="C53" s="2">
         <v>0</v>
@@ -3663,15 +3672,15 @@
         <v>0</v>
       </c>
       <c r="H53" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
-        <v>498</v>
+        <v>488</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C54" s="2">
         <v>0</v>
@@ -3689,15 +3698,15 @@
         <v>0</v>
       </c>
       <c r="H54" s="9" t="s">
-        <v>500</v>
+        <v>490</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
-        <v>374</v>
+        <v>498</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>40</v>
+        <v>499</v>
       </c>
       <c r="C55" s="2">
         <v>0</v>
@@ -3715,15 +3724,15 @@
         <v>0</v>
       </c>
       <c r="H55" s="9" t="s">
-        <v>211</v>
+        <v>500</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C56" s="2">
         <v>0</v>
@@ -3741,15 +3750,15 @@
         <v>0</v>
       </c>
       <c r="H56" s="9" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C57" s="2">
         <v>0</v>
@@ -3767,119 +3776,119 @@
         <v>0</v>
       </c>
       <c r="H57" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C58" s="2">
+        <v>0</v>
+      </c>
+      <c r="D58" s="2">
+        <v>1</v>
+      </c>
+      <c r="E58" s="4">
+        <v>0</v>
+      </c>
+      <c r="F58" s="4">
+        <v>0</v>
+      </c>
+      <c r="G58" s="3">
+        <v>0</v>
+      </c>
+      <c r="H58" s="9" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="9" t="s">
         <v>377</v>
       </c>
-      <c r="B58" s="9" t="s">
+      <c r="B59" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C58" s="2">
-        <v>0</v>
-      </c>
-      <c r="D58" s="2">
-        <v>1</v>
-      </c>
-      <c r="E58" s="4">
-        <v>0</v>
-      </c>
-      <c r="F58" s="4">
-        <v>0</v>
-      </c>
-      <c r="G58" s="3">
-        <v>0</v>
-      </c>
-      <c r="H58" s="9" t="s">
+      <c r="C59" s="2">
+        <v>0</v>
+      </c>
+      <c r="D59" s="2">
+        <v>1</v>
+      </c>
+      <c r="E59" s="4">
+        <v>0</v>
+      </c>
+      <c r="F59" s="4">
+        <v>0</v>
+      </c>
+      <c r="G59" s="3">
+        <v>0</v>
+      </c>
+      <c r="H59" s="9" t="s">
         <v>216</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="19" t="s">
-        <v>503</v>
-      </c>
-      <c r="B59" s="19" t="s">
-        <v>504</v>
-      </c>
-      <c r="C59" s="2">
-        <v>1</v>
-      </c>
-      <c r="D59" s="2">
-        <v>1</v>
-      </c>
-      <c r="E59" s="4">
-        <v>1</v>
-      </c>
-      <c r="F59" s="4">
-        <v>1</v>
-      </c>
-      <c r="G59" s="3">
-        <v>1</v>
-      </c>
-      <c r="H59" s="11" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="19" t="s">
+        <v>503</v>
+      </c>
+      <c r="B60" s="19" t="s">
+        <v>504</v>
+      </c>
+      <c r="C60" s="2">
+        <v>1</v>
+      </c>
+      <c r="D60" s="2">
+        <v>1</v>
+      </c>
+      <c r="E60" s="4">
+        <v>1</v>
+      </c>
+      <c r="F60" s="4">
+        <v>1</v>
+      </c>
+      <c r="G60" s="3">
+        <v>1</v>
+      </c>
+      <c r="H60" s="11" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="19" t="s">
         <v>505</v>
       </c>
-      <c r="B60" s="19" t="s">
+      <c r="B61" s="19" t="s">
         <v>506</v>
       </c>
-      <c r="C60" s="2">
-        <v>1</v>
-      </c>
-      <c r="D60" s="2">
-        <v>1</v>
-      </c>
-      <c r="E60" s="4">
-        <v>1</v>
-      </c>
-      <c r="F60" s="4">
-        <v>1</v>
-      </c>
-      <c r="G60" s="3">
-        <v>1</v>
-      </c>
-      <c r="H60" s="11" t="s">
+      <c r="C61" s="2">
+        <v>1</v>
+      </c>
+      <c r="D61" s="2">
+        <v>1</v>
+      </c>
+      <c r="E61" s="4">
+        <v>1</v>
+      </c>
+      <c r="F61" s="4">
+        <v>1</v>
+      </c>
+      <c r="G61" s="3">
+        <v>1</v>
+      </c>
+      <c r="H61" s="11" t="s">
         <v>506</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="11" t="s">
-        <v>598</v>
-      </c>
-      <c r="B61" s="11" t="s">
-        <v>502</v>
-      </c>
-      <c r="C61" s="2">
-        <v>1</v>
-      </c>
-      <c r="D61" s="2">
-        <v>1</v>
-      </c>
-      <c r="E61" s="4">
-        <v>1</v>
-      </c>
-      <c r="F61" s="4">
-        <v>0</v>
-      </c>
-      <c r="G61" s="3">
-        <v>1</v>
-      </c>
-      <c r="H61" s="11" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>600</v>
+        <v>502</v>
       </c>
       <c r="C62" s="2">
         <v>1</v>
@@ -3901,45 +3910,45 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="13" t="s">
-        <v>378</v>
-      </c>
-      <c r="B63" s="13" t="s">
-        <v>51</v>
+      <c r="A63" s="11" t="s">
+        <v>599</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>600</v>
       </c>
       <c r="C63" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D63" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E63" s="4">
         <v>1</v>
       </c>
-      <c r="F63" s="3">
+      <c r="F63" s="4">
         <v>0</v>
       </c>
       <c r="G63" s="3">
         <v>1</v>
       </c>
-      <c r="H63" s="13" t="s">
-        <v>217</v>
+      <c r="H63" s="11" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="13" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C64" s="20">
-        <v>0</v>
-      </c>
-      <c r="D64" s="20">
-        <v>0</v>
-      </c>
-      <c r="E64" s="21">
+        <v>51</v>
+      </c>
+      <c r="C64" s="2">
+        <v>0</v>
+      </c>
+      <c r="D64" s="2">
+        <v>0</v>
+      </c>
+      <c r="E64" s="4">
         <v>1</v>
       </c>
       <c r="F64" s="3">
@@ -3949,15 +3958,15 @@
         <v>1</v>
       </c>
       <c r="H64" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="13" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C65" s="20">
         <v>0</v>
@@ -3965,7 +3974,7 @@
       <c r="D65" s="20">
         <v>0</v>
       </c>
-      <c r="E65" s="20">
+      <c r="E65" s="21">
         <v>1</v>
       </c>
       <c r="F65" s="3">
@@ -3975,15 +3984,15 @@
         <v>1</v>
       </c>
       <c r="H65" s="13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="13" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C66" s="20">
         <v>0</v>
@@ -3991,7 +4000,7 @@
       <c r="D66" s="20">
         <v>0</v>
       </c>
-      <c r="E66" s="21">
+      <c r="E66" s="20">
         <v>1</v>
       </c>
       <c r="F66" s="3">
@@ -4001,15 +4010,15 @@
         <v>1</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="13" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C67" s="20">
         <v>0</v>
@@ -4027,23 +4036,23 @@
         <v>1</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="13" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C68" s="2">
-        <v>0</v>
-      </c>
-      <c r="D68" s="2">
-        <v>0</v>
-      </c>
-      <c r="E68" s="4">
+        <v>55</v>
+      </c>
+      <c r="C68" s="20">
+        <v>0</v>
+      </c>
+      <c r="D68" s="20">
+        <v>0</v>
+      </c>
+      <c r="E68" s="21">
         <v>1</v>
       </c>
       <c r="F68" s="3">
@@ -4053,15 +4062,15 @@
         <v>1</v>
       </c>
       <c r="H68" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C69" s="2">
         <v>0</v>
@@ -4079,15 +4088,15 @@
         <v>1</v>
       </c>
       <c r="H69" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="13" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C70" s="2">
         <v>0</v>
@@ -4105,15 +4114,15 @@
         <v>1</v>
       </c>
       <c r="H70" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="13" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C71" s="2">
         <v>0</v>
@@ -4131,15 +4140,15 @@
         <v>1</v>
       </c>
       <c r="H71" s="13" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="13" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C72" s="2">
         <v>0</v>
@@ -4157,15 +4166,15 @@
         <v>1</v>
       </c>
       <c r="H72" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="13" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C73" s="2">
         <v>0</v>
@@ -4183,15 +4192,15 @@
         <v>1</v>
       </c>
       <c r="H73" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="13" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C74" s="2">
         <v>0</v>
@@ -4209,15 +4218,15 @@
         <v>1</v>
       </c>
       <c r="H74" s="13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="13" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C75" s="2">
         <v>0</v>
@@ -4235,15 +4244,15 @@
         <v>1</v>
       </c>
       <c r="H75" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="13" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C76" s="2">
         <v>0</v>
@@ -4261,15 +4270,15 @@
         <v>1</v>
       </c>
       <c r="H76" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="13" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C77" s="2">
         <v>0</v>
@@ -4287,15 +4296,15 @@
         <v>1</v>
       </c>
       <c r="H77" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="13" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C78" s="2">
         <v>0</v>
@@ -4313,15 +4322,15 @@
         <v>1</v>
       </c>
       <c r="H78" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="13" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C79" s="2">
         <v>0</v>
@@ -4339,15 +4348,15 @@
         <v>1</v>
       </c>
       <c r="H79" s="13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="13" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C80" s="2">
         <v>0</v>
@@ -4365,15 +4374,15 @@
         <v>1</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="13" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C81" s="2">
         <v>0</v>
@@ -4391,15 +4400,15 @@
         <v>1</v>
       </c>
       <c r="H81" s="13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="13" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C82" s="2">
         <v>0</v>
@@ -4417,23 +4426,23 @@
         <v>1</v>
       </c>
       <c r="H82" s="13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="13" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="C83" s="20">
+        <v>70</v>
+      </c>
+      <c r="C83" s="2">
         <v>0</v>
       </c>
       <c r="D83" s="2">
         <v>0</v>
       </c>
-      <c r="E83" s="21">
+      <c r="E83" s="4">
         <v>1</v>
       </c>
       <c r="F83" s="3">
@@ -4443,15 +4452,15 @@
         <v>1</v>
       </c>
       <c r="H83" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="13" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B84" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C84" s="20">
         <v>0</v>
@@ -4459,7 +4468,7 @@
       <c r="D84" s="2">
         <v>0</v>
       </c>
-      <c r="E84" s="20">
+      <c r="E84" s="21">
         <v>1</v>
       </c>
       <c r="F84" s="3">
@@ -4469,15 +4478,15 @@
         <v>1</v>
       </c>
       <c r="H84" s="13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="13" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C85" s="20">
         <v>0</v>
@@ -4485,7 +4494,7 @@
       <c r="D85" s="2">
         <v>0</v>
       </c>
-      <c r="E85" s="21">
+      <c r="E85" s="20">
         <v>1</v>
       </c>
       <c r="F85" s="3">
@@ -4495,15 +4504,15 @@
         <v>1</v>
       </c>
       <c r="H85" s="13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="13" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B86" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C86" s="20">
         <v>0</v>
@@ -4521,15 +4530,15 @@
         <v>1</v>
       </c>
       <c r="H86" s="13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="13" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B87" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C87" s="20">
         <v>0</v>
@@ -4537,7 +4546,7 @@
       <c r="D87" s="2">
         <v>0</v>
       </c>
-      <c r="E87" s="20">
+      <c r="E87" s="21">
         <v>1</v>
       </c>
       <c r="F87" s="3">
@@ -4547,15 +4556,15 @@
         <v>1</v>
       </c>
       <c r="H87" s="13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="13" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B88" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C88" s="20">
         <v>0</v>
@@ -4563,7 +4572,7 @@
       <c r="D88" s="2">
         <v>0</v>
       </c>
-      <c r="E88" s="4">
+      <c r="E88" s="20">
         <v>1</v>
       </c>
       <c r="F88" s="3">
@@ -4573,15 +4582,15 @@
         <v>1</v>
       </c>
       <c r="H88" s="13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="13" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C89" s="20">
         <v>0</v>
@@ -4599,17 +4608,17 @@
         <v>1</v>
       </c>
       <c r="H89" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="13" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B90" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C90" s="2">
+        <v>77</v>
+      </c>
+      <c r="C90" s="20">
         <v>0</v>
       </c>
       <c r="D90" s="2">
@@ -4625,67 +4634,67 @@
         <v>1</v>
       </c>
       <c r="H90" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="13" t="s">
+        <v>405</v>
+      </c>
+      <c r="B91" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C91" s="2">
+        <v>0</v>
+      </c>
+      <c r="D91" s="2">
+        <v>0</v>
+      </c>
+      <c r="E91" s="4">
+        <v>1</v>
+      </c>
+      <c r="F91" s="3">
+        <v>0</v>
+      </c>
+      <c r="G91" s="3">
+        <v>1</v>
+      </c>
+      <c r="H91" s="13" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="13" t="s">
         <v>406</v>
       </c>
-      <c r="B91" s="13" t="s">
+      <c r="B92" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C91" s="2">
-        <v>0</v>
-      </c>
-      <c r="D91" s="2">
-        <v>0</v>
-      </c>
-      <c r="E91" s="4">
-        <v>1</v>
-      </c>
-      <c r="F91" s="3">
-        <v>0</v>
-      </c>
-      <c r="G91" s="3">
-        <v>1</v>
-      </c>
-      <c r="H91" s="13" t="s">
+      <c r="C92" s="2">
+        <v>0</v>
+      </c>
+      <c r="D92" s="2">
+        <v>0</v>
+      </c>
+      <c r="E92" s="4">
+        <v>1</v>
+      </c>
+      <c r="F92" s="3">
+        <v>0</v>
+      </c>
+      <c r="G92" s="3">
+        <v>1</v>
+      </c>
+      <c r="H92" s="13" t="s">
         <v>257</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A92" s="17" t="s">
-        <v>407</v>
-      </c>
-      <c r="B92" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C92" s="2">
-        <v>0</v>
-      </c>
-      <c r="D92" s="2">
-        <v>0</v>
-      </c>
-      <c r="E92" s="2">
-        <v>1</v>
-      </c>
-      <c r="F92" s="3">
-        <v>1</v>
-      </c>
-      <c r="G92" s="3">
-        <v>1</v>
-      </c>
-      <c r="H92" s="17" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="17" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B93" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C93" s="2">
         <v>0</v>
@@ -4700,18 +4709,18 @@
         <v>1</v>
       </c>
       <c r="G93" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H93" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="17" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B94" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C94" s="2">
         <v>0</v>
@@ -4729,15 +4738,15 @@
         <v>0</v>
       </c>
       <c r="H94" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="17" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B95" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C95" s="2">
         <v>0</v>
@@ -4755,15 +4764,15 @@
         <v>0</v>
       </c>
       <c r="H95" s="17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="17" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B96" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C96" s="2">
         <v>0</v>
@@ -4781,15 +4790,15 @@
         <v>0</v>
       </c>
       <c r="H96" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="17" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B97" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C97" s="2">
         <v>0</v>
@@ -4807,15 +4816,15 @@
         <v>0</v>
       </c>
       <c r="H97" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="17" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B98" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C98" s="2">
         <v>0</v>
@@ -4833,15 +4842,15 @@
         <v>0</v>
       </c>
       <c r="H98" s="17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="17" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B99" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C99" s="2">
         <v>0</v>
@@ -4859,15 +4868,15 @@
         <v>0</v>
       </c>
       <c r="H99" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="17" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B100" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C100" s="2">
         <v>0</v>
@@ -4885,15 +4894,15 @@
         <v>0</v>
       </c>
       <c r="H100" s="17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="17" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B101" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C101" s="2">
         <v>0</v>
@@ -4911,15 +4920,15 @@
         <v>0</v>
       </c>
       <c r="H101" s="17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="17" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B102" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C102" s="2">
         <v>0</v>
@@ -4937,15 +4946,15 @@
         <v>0</v>
       </c>
       <c r="H102" s="17" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B103" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C103" s="2">
         <v>0</v>
@@ -4963,15 +4972,15 @@
         <v>0</v>
       </c>
       <c r="H103" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="17" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B104" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C104" s="2">
         <v>0</v>
@@ -4989,15 +4998,15 @@
         <v>0</v>
       </c>
       <c r="H104" s="17" t="s">
-        <v>258</v>
+        <v>236</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="17" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B105" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C105" s="2">
         <v>0</v>
@@ -5015,15 +5024,15 @@
         <v>0</v>
       </c>
       <c r="H105" s="17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="17" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B106" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C106" s="2">
         <v>0</v>
@@ -5041,15 +5050,15 @@
         <v>0</v>
       </c>
       <c r="H106" s="17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="17" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B107" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C107" s="2">
         <v>0</v>
@@ -5067,15 +5076,15 @@
         <v>0</v>
       </c>
       <c r="H107" s="17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="17" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B108" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C108" s="2">
         <v>0</v>
@@ -5093,15 +5102,15 @@
         <v>0</v>
       </c>
       <c r="H108" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="17" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B109" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C109" s="2">
         <v>0</v>
@@ -5116,18 +5125,18 @@
         <v>1</v>
       </c>
       <c r="G109" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H109" s="17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="17" t="s">
-        <v>426</v>
-      </c>
-      <c r="B110" s="15" t="s">
-        <v>98</v>
+        <v>425</v>
+      </c>
+      <c r="B110" s="14" t="s">
+        <v>97</v>
       </c>
       <c r="C110" s="2">
         <v>0</v>
@@ -5145,15 +5154,15 @@
         <v>1</v>
       </c>
       <c r="H110" s="17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="17" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B111" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C111" s="2">
         <v>0</v>
@@ -5171,15 +5180,15 @@
         <v>1</v>
       </c>
       <c r="H111" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" s="17" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B112" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C112" s="2">
         <v>0</v>
@@ -5197,15 +5206,15 @@
         <v>1</v>
       </c>
       <c r="H112" s="17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" s="17" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B113" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C113" s="2">
         <v>0</v>
@@ -5223,15 +5232,15 @@
         <v>1</v>
       </c>
       <c r="H113" s="17" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" s="17" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B114" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C114" s="2">
         <v>0</v>
@@ -5249,15 +5258,15 @@
         <v>1</v>
       </c>
       <c r="H114" s="17" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="17" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B115" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C115" s="2">
         <v>0</v>
@@ -5275,15 +5284,15 @@
         <v>1</v>
       </c>
       <c r="H115" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" s="17" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B116" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C116" s="2">
         <v>0</v>
@@ -5301,15 +5310,15 @@
         <v>1</v>
       </c>
       <c r="H116" s="17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" s="17" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B117" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C117" s="2">
         <v>0</v>
@@ -5317,25 +5326,25 @@
       <c r="D117" s="2">
         <v>0</v>
       </c>
-      <c r="E117" s="20">
-        <v>1</v>
-      </c>
-      <c r="F117" s="22">
+      <c r="E117" s="2">
+        <v>1</v>
+      </c>
+      <c r="F117" s="3">
         <v>1</v>
       </c>
       <c r="G117" s="3">
         <v>1</v>
       </c>
       <c r="H117" s="17" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" s="17" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B118" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C118" s="2">
         <v>0</v>
@@ -5353,15 +5362,15 @@
         <v>1</v>
       </c>
       <c r="H118" s="17" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" s="17" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B119" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C119" s="2">
         <v>0</v>
@@ -5379,15 +5388,15 @@
         <v>1</v>
       </c>
       <c r="H119" s="17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" s="17" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B120" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C120" s="2">
         <v>0</v>
@@ -5398,22 +5407,22 @@
       <c r="E120" s="20">
         <v>1</v>
       </c>
-      <c r="F120" s="20">
+      <c r="F120" s="22">
         <v>1</v>
       </c>
       <c r="G120" s="3">
         <v>1</v>
       </c>
       <c r="H120" s="17" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" s="17" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B121" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C121" s="2">
         <v>0</v>
@@ -5424,22 +5433,22 @@
       <c r="E121" s="20">
         <v>1</v>
       </c>
-      <c r="F121" s="22">
+      <c r="F121" s="20">
         <v>1</v>
       </c>
       <c r="G121" s="3">
         <v>1</v>
       </c>
       <c r="H121" s="17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" s="17" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B122" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C122" s="2">
         <v>0</v>
@@ -5457,15 +5466,15 @@
         <v>1</v>
       </c>
       <c r="H122" s="17" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" s="17" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B123" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C123" s="2">
         <v>0</v>
@@ -5483,15 +5492,15 @@
         <v>1</v>
       </c>
       <c r="H123" s="17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" s="17" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B124" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C124" s="2">
         <v>0</v>
@@ -5502,22 +5511,22 @@
       <c r="E124" s="20">
         <v>1</v>
       </c>
-      <c r="F124" s="20">
+      <c r="F124" s="22">
         <v>1</v>
       </c>
       <c r="G124" s="3">
         <v>1</v>
       </c>
       <c r="H124" s="17" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" s="17" t="s">
-        <v>441</v>
-      </c>
-      <c r="B125" s="14" t="s">
-        <v>113</v>
+        <v>440</v>
+      </c>
+      <c r="B125" s="15" t="s">
+        <v>112</v>
       </c>
       <c r="C125" s="2">
         <v>0</v>
@@ -5528,22 +5537,22 @@
       <c r="E125" s="20">
         <v>1</v>
       </c>
-      <c r="F125" s="22">
+      <c r="F125" s="20">
         <v>1</v>
       </c>
       <c r="G125" s="3">
         <v>1</v>
       </c>
       <c r="H125" s="17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" s="17" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B126" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C126" s="2">
         <v>0</v>
@@ -5558,18 +5567,18 @@
         <v>1</v>
       </c>
       <c r="G126" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H126" s="17" t="s">
-        <v>114</v>
+        <v>279</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" s="17" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B127" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C127" s="2">
         <v>0</v>
@@ -5587,15 +5596,15 @@
         <v>0</v>
       </c>
       <c r="H127" s="17" t="s">
-        <v>280</v>
+        <v>114</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" s="17" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B128" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C128" s="2">
         <v>0</v>
@@ -5613,15 +5622,15 @@
         <v>0</v>
       </c>
       <c r="H128" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" s="17" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B129" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C129" s="2">
         <v>0</v>
@@ -5639,15 +5648,15 @@
         <v>0</v>
       </c>
       <c r="H129" s="17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" s="17" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B130" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C130" s="2">
         <v>0</v>
@@ -5658,22 +5667,22 @@
       <c r="E130" s="20">
         <v>1</v>
       </c>
-      <c r="F130" s="20">
+      <c r="F130" s="22">
         <v>1</v>
       </c>
       <c r="G130" s="3">
         <v>0</v>
       </c>
       <c r="H130" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" s="17" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B131" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C131" s="2">
         <v>0</v>
@@ -5684,22 +5693,22 @@
       <c r="E131" s="20">
         <v>1</v>
       </c>
-      <c r="F131" s="22">
+      <c r="F131" s="20">
         <v>1</v>
       </c>
       <c r="G131" s="3">
         <v>0</v>
       </c>
       <c r="H131" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" s="17" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B132" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C132" s="2">
         <v>0</v>
@@ -5717,67 +5726,67 @@
         <v>0</v>
       </c>
       <c r="H132" s="17" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" s="17" t="s">
+        <v>448</v>
+      </c>
+      <c r="B133" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C133" s="2">
+        <v>0</v>
+      </c>
+      <c r="D133" s="2">
+        <v>0</v>
+      </c>
+      <c r="E133" s="20">
+        <v>1</v>
+      </c>
+      <c r="F133" s="22">
+        <v>1</v>
+      </c>
+      <c r="G133" s="3">
+        <v>0</v>
+      </c>
+      <c r="H133" s="17" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A134" s="17" t="s">
         <v>449</v>
       </c>
-      <c r="B133" s="14" t="s">
+      <c r="B134" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="C133" s="2">
-        <v>0</v>
-      </c>
-      <c r="D133" s="2">
-        <v>0</v>
-      </c>
-      <c r="E133" s="20">
-        <v>1</v>
-      </c>
-      <c r="F133" s="22">
-        <v>1</v>
-      </c>
-      <c r="G133" s="3">
-        <v>0</v>
-      </c>
-      <c r="H133" s="17" t="s">
+      <c r="C134" s="2">
+        <v>0</v>
+      </c>
+      <c r="D134" s="2">
+        <v>0</v>
+      </c>
+      <c r="E134" s="20">
+        <v>1</v>
+      </c>
+      <c r="F134" s="22">
+        <v>1</v>
+      </c>
+      <c r="G134" s="3">
+        <v>0</v>
+      </c>
+      <c r="H134" s="17" t="s">
         <v>286</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A134" s="18" t="s">
-        <v>574</v>
-      </c>
-      <c r="B134" s="16" t="s">
-        <v>580</v>
-      </c>
-      <c r="C134" s="2">
-        <v>0</v>
-      </c>
-      <c r="D134" s="2">
-        <v>0</v>
-      </c>
-      <c r="E134" s="20">
-        <v>1</v>
-      </c>
-      <c r="F134" s="20">
-        <v>1</v>
-      </c>
-      <c r="G134" s="3">
-        <v>0</v>
-      </c>
-      <c r="H134" s="18" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" s="18" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B135" s="16" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C135" s="2">
         <v>0</v>
@@ -5795,15 +5804,15 @@
         <v>0</v>
       </c>
       <c r="H135" s="18" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" s="18" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B136" s="16" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C136" s="2">
         <v>0</v>
@@ -5821,15 +5830,15 @@
         <v>0</v>
       </c>
       <c r="H136" s="18" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" s="18" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B137" s="16" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C137" s="2">
         <v>0</v>
@@ -5847,15 +5856,15 @@
         <v>0</v>
       </c>
       <c r="H137" s="18" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" s="18" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B138" s="16" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C138" s="2">
         <v>0</v>
@@ -5873,67 +5882,67 @@
         <v>0</v>
       </c>
       <c r="H138" s="18" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" s="18" t="s">
+        <v>578</v>
+      </c>
+      <c r="B139" s="16" t="s">
+        <v>584</v>
+      </c>
+      <c r="C139" s="2">
+        <v>0</v>
+      </c>
+      <c r="D139" s="2">
+        <v>0</v>
+      </c>
+      <c r="E139" s="20">
+        <v>1</v>
+      </c>
+      <c r="F139" s="20">
+        <v>1</v>
+      </c>
+      <c r="G139" s="3">
+        <v>0</v>
+      </c>
+      <c r="H139" s="18" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A140" s="18" t="s">
         <v>579</v>
       </c>
-      <c r="B139" s="16" t="s">
+      <c r="B140" s="16" t="s">
         <v>585</v>
       </c>
-      <c r="C139" s="2">
-        <v>0</v>
-      </c>
-      <c r="D139" s="2">
-        <v>0</v>
-      </c>
-      <c r="E139" s="20">
-        <v>1</v>
-      </c>
-      <c r="F139" s="20">
-        <v>1</v>
-      </c>
-      <c r="G139" s="3">
-        <v>0</v>
-      </c>
-      <c r="H139" s="18" t="s">
+      <c r="C140" s="2">
+        <v>0</v>
+      </c>
+      <c r="D140" s="2">
+        <v>0</v>
+      </c>
+      <c r="E140" s="20">
+        <v>1</v>
+      </c>
+      <c r="F140" s="20">
+        <v>1</v>
+      </c>
+      <c r="G140" s="3">
+        <v>0</v>
+      </c>
+      <c r="H140" s="18" t="s">
         <v>555</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A140" s="17" t="s">
-        <v>450</v>
-      </c>
-      <c r="B140" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="C140" s="2">
-        <v>0</v>
-      </c>
-      <c r="D140" s="2">
-        <v>0</v>
-      </c>
-      <c r="E140" s="20">
-        <v>1</v>
-      </c>
-      <c r="F140" s="22">
-        <v>1</v>
-      </c>
-      <c r="G140" s="3">
-        <v>0</v>
-      </c>
-      <c r="H140" s="17" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" s="17" t="s">
-        <v>556</v>
-      </c>
-      <c r="B141" s="23" t="s">
-        <v>532</v>
+        <v>450</v>
+      </c>
+      <c r="B141" s="14" t="s">
+        <v>122</v>
       </c>
       <c r="C141" s="2">
         <v>0</v>
@@ -5941,7 +5950,7 @@
       <c r="D141" s="2">
         <v>0</v>
       </c>
-      <c r="E141" s="4">
+      <c r="E141" s="20">
         <v>1</v>
       </c>
       <c r="F141" s="22">
@@ -5951,15 +5960,15 @@
         <v>0</v>
       </c>
       <c r="H141" s="17" t="s">
-        <v>514</v>
+        <v>287</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" s="17" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B142" s="23" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C142" s="2">
         <v>0</v>
@@ -5977,15 +5986,15 @@
         <v>0</v>
       </c>
       <c r="H142" s="17" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" s="17" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B143" s="23" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="C143" s="2">
         <v>0</v>
@@ -6003,15 +6012,15 @@
         <v>0</v>
       </c>
       <c r="H143" s="17" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" s="17" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B144" s="23" t="s">
-        <v>534</v>
+        <v>539</v>
       </c>
       <c r="C144" s="2">
         <v>0</v>
@@ -6029,15 +6038,15 @@
         <v>0</v>
       </c>
       <c r="H144" s="17" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" s="17" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B145" s="23" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="C145" s="2">
         <v>0</v>
@@ -6055,15 +6064,15 @@
         <v>0</v>
       </c>
       <c r="H145" s="17" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" s="17" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B146" s="23" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C146" s="2">
         <v>0</v>
@@ -6081,15 +6090,15 @@
         <v>0</v>
       </c>
       <c r="H146" s="17" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" s="17" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B147" s="23" t="s">
-        <v>535</v>
+        <v>541</v>
       </c>
       <c r="C147" s="2">
         <v>0</v>
@@ -6107,15 +6116,15 @@
         <v>0</v>
       </c>
       <c r="H147" s="17" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" s="17" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B148" s="23" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="C148" s="2">
         <v>0</v>
@@ -6133,15 +6142,15 @@
         <v>0</v>
       </c>
       <c r="H148" s="17" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" s="17" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B149" s="23" t="s">
-        <v>536</v>
+        <v>542</v>
       </c>
       <c r="C149" s="2">
         <v>0</v>
@@ -6159,15 +6168,15 @@
         <v>0</v>
       </c>
       <c r="H149" s="17" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" s="17" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B150" s="23" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="C150" s="2">
         <v>0</v>
@@ -6185,15 +6194,15 @@
         <v>0</v>
       </c>
       <c r="H150" s="17" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" s="17" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B151" s="23" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C151" s="2">
         <v>0</v>
@@ -6211,15 +6220,15 @@
         <v>0</v>
       </c>
       <c r="H151" s="17" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" s="17" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B152" s="23" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C152" s="2">
         <v>0</v>
@@ -6237,15 +6246,15 @@
         <v>0</v>
       </c>
       <c r="H152" s="17" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" s="17" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B153" s="23" t="s">
-        <v>537</v>
+        <v>545</v>
       </c>
       <c r="C153" s="2">
         <v>0</v>
@@ -6263,15 +6272,15 @@
         <v>0</v>
       </c>
       <c r="H153" s="17" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" s="17" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B154" s="23" t="s">
-        <v>546</v>
+        <v>537</v>
       </c>
       <c r="C154" s="2">
         <v>0</v>
@@ -6289,15 +6298,15 @@
         <v>0</v>
       </c>
       <c r="H154" s="17" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" s="17" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B155" s="23" t="s">
-        <v>538</v>
+        <v>546</v>
       </c>
       <c r="C155" s="2">
         <v>0</v>
@@ -6315,15 +6324,15 @@
         <v>0</v>
       </c>
       <c r="H155" s="17" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" s="17" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B156" s="23" t="s">
-        <v>547</v>
+        <v>538</v>
       </c>
       <c r="C156" s="2">
         <v>0</v>
@@ -6341,15 +6350,15 @@
         <v>0</v>
       </c>
       <c r="H156" s="17" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" s="17" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B157" s="23" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C157" s="2">
         <v>0</v>
@@ -6367,15 +6376,15 @@
         <v>0</v>
       </c>
       <c r="H157" s="17" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" s="17" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B158" s="23" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="C158" s="2">
         <v>0</v>
@@ -6393,15 +6402,15 @@
         <v>0</v>
       </c>
       <c r="H158" s="17" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" s="17" t="s">
-        <v>451</v>
-      </c>
-      <c r="B159" s="14" t="s">
-        <v>123</v>
+        <v>573</v>
+      </c>
+      <c r="B159" s="23" t="s">
+        <v>548</v>
       </c>
       <c r="C159" s="2">
         <v>0</v>
@@ -6409,7 +6418,7 @@
       <c r="D159" s="2">
         <v>0</v>
       </c>
-      <c r="E159" s="20">
+      <c r="E159" s="4">
         <v>1</v>
       </c>
       <c r="F159" s="22">
@@ -6419,15 +6428,15 @@
         <v>0</v>
       </c>
       <c r="H159" s="17" t="s">
-        <v>288</v>
+        <v>531</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" s="17" t="s">
-        <v>416</v>
+        <v>451</v>
       </c>
       <c r="B160" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C160" s="2">
         <v>0</v>
@@ -6445,15 +6454,15 @@
         <v>0</v>
       </c>
       <c r="H160" s="17" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" s="17" t="s">
-        <v>452</v>
+        <v>416</v>
       </c>
       <c r="B161" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C161" s="2">
         <v>0</v>
@@ -6468,18 +6477,18 @@
         <v>1</v>
       </c>
       <c r="G161" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H161" s="17" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" s="17" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B162" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C162" s="2">
         <v>0</v>
@@ -6497,15 +6506,15 @@
         <v>1</v>
       </c>
       <c r="H162" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" s="17" t="s">
-        <v>602</v>
+        <v>453</v>
       </c>
       <c r="B163" s="14" t="s">
-        <v>603</v>
+        <v>126</v>
       </c>
       <c r="C163" s="2">
         <v>0</v>
@@ -6523,15 +6532,15 @@
         <v>1</v>
       </c>
       <c r="H163" s="17" t="s">
-        <v>604</v>
+        <v>291</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" s="17" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="B164" s="14" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="C164" s="2">
         <v>0</v>
@@ -6549,15 +6558,15 @@
         <v>1</v>
       </c>
       <c r="H164" s="17" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" s="17" t="s">
-        <v>454</v>
-      </c>
-      <c r="B165" s="15" t="s">
-        <v>127</v>
+        <v>605</v>
+      </c>
+      <c r="B165" s="14" t="s">
+        <v>606</v>
       </c>
       <c r="C165" s="2">
         <v>0</v>
@@ -6572,18 +6581,18 @@
         <v>1</v>
       </c>
       <c r="G165" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H165" s="17" t="s">
-        <v>292</v>
+        <v>607</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" s="17" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B166" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C166" s="2">
         <v>0</v>
@@ -6601,15 +6610,15 @@
         <v>0</v>
       </c>
       <c r="H166" s="17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" s="17" t="s">
-        <v>456</v>
-      </c>
-      <c r="B167" s="14" t="s">
-        <v>129</v>
+        <v>455</v>
+      </c>
+      <c r="B167" s="15" t="s">
+        <v>128</v>
       </c>
       <c r="C167" s="2">
         <v>0</v>
@@ -6627,15 +6636,15 @@
         <v>0</v>
       </c>
       <c r="H167" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" s="17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B168" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C168" s="2">
         <v>0</v>
@@ -6646,22 +6655,22 @@
       <c r="E168" s="20">
         <v>1</v>
       </c>
-      <c r="F168" s="20">
+      <c r="F168" s="22">
         <v>1</v>
       </c>
       <c r="G168" s="3">
         <v>0</v>
       </c>
       <c r="H168" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" s="17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B169" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C169" s="2">
         <v>0</v>
@@ -6672,22 +6681,22 @@
       <c r="E169" s="20">
         <v>1</v>
       </c>
-      <c r="F169" s="22">
+      <c r="F169" s="20">
         <v>1</v>
       </c>
       <c r="G169" s="3">
         <v>0</v>
       </c>
       <c r="H169" s="17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" s="17" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B170" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C170" s="2">
         <v>0</v>
@@ -6705,15 +6714,15 @@
         <v>0</v>
       </c>
       <c r="H170" s="17" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" s="17" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B171" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C171" s="2">
         <v>0</v>
@@ -6728,18 +6737,18 @@
         <v>1</v>
       </c>
       <c r="G171" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H171" s="17" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" s="17" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B172" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C172" s="2">
         <v>0</v>
@@ -6757,15 +6766,15 @@
         <v>1</v>
       </c>
       <c r="H172" s="17" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" s="17" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B173" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C173" s="2">
         <v>0</v>
@@ -6780,18 +6789,18 @@
         <v>1</v>
       </c>
       <c r="G173" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H173" s="17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" s="17" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B174" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C174" s="2">
         <v>0</v>
@@ -6809,15 +6818,15 @@
         <v>0</v>
       </c>
       <c r="H174" s="17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" s="17" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B175" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C175" s="2">
         <v>0</v>
@@ -6835,15 +6844,15 @@
         <v>0</v>
       </c>
       <c r="H175" s="17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" s="17" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B176" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C176" s="2">
         <v>0</v>
@@ -6861,15 +6870,15 @@
         <v>0</v>
       </c>
       <c r="H176" s="17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" s="17" t="s">
-        <v>586</v>
+        <v>465</v>
       </c>
       <c r="B177" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C177" s="2">
         <v>0</v>
@@ -6887,15 +6896,15 @@
         <v>0</v>
       </c>
       <c r="H177" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" s="17" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B178" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C178" s="2">
         <v>0</v>
@@ -6913,15 +6922,15 @@
         <v>0</v>
       </c>
       <c r="H178" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" s="17" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="B179" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C179" s="2">
         <v>0</v>
@@ -6939,15 +6948,15 @@
         <v>0</v>
       </c>
       <c r="H179" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" s="17" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B180" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C180" s="2">
         <v>0</v>
@@ -6965,15 +6974,15 @@
         <v>0</v>
       </c>
       <c r="H180" s="17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" s="17" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B181" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C181" s="2">
         <v>0</v>
@@ -6991,15 +7000,15 @@
         <v>0</v>
       </c>
       <c r="H181" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" s="17" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B182" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C182" s="2">
         <v>0</v>
@@ -7017,15 +7026,15 @@
         <v>0</v>
       </c>
       <c r="H182" s="17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" s="17" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B183" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C183" s="2">
         <v>0</v>
@@ -7043,15 +7052,15 @@
         <v>0</v>
       </c>
       <c r="H183" s="17" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" s="17" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B184" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C184" s="2">
         <v>0</v>
@@ -7069,15 +7078,15 @@
         <v>0</v>
       </c>
       <c r="H184" s="17" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" s="17" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B185" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C185" s="2">
         <v>0</v>
@@ -7095,15 +7104,15 @@
         <v>0</v>
       </c>
       <c r="H185" s="17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" s="17" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B186" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C186" s="2">
         <v>0</v>
@@ -7121,15 +7130,15 @@
         <v>0</v>
       </c>
       <c r="H186" s="17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" s="17" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B187" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C187" s="2">
         <v>0</v>
@@ -7147,15 +7156,15 @@
         <v>0</v>
       </c>
       <c r="H187" s="17" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" s="17" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B188" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C188" s="2">
         <v>0</v>
@@ -7173,15 +7182,15 @@
         <v>0</v>
       </c>
       <c r="H188" s="17" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" s="17" t="s">
-        <v>466</v>
+        <v>597</v>
       </c>
       <c r="B189" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C189" s="2">
         <v>0</v>
@@ -7199,15 +7208,15 @@
         <v>0</v>
       </c>
       <c r="H189" s="17" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" s="17" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B190" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C190" s="2">
         <v>0</v>
@@ -7218,22 +7227,22 @@
       <c r="E190" s="20">
         <v>1</v>
       </c>
-      <c r="F190" s="20">
+      <c r="F190" s="22">
         <v>1</v>
       </c>
       <c r="G190" s="3">
         <v>0</v>
       </c>
       <c r="H190" s="17" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B191" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C191" s="2">
         <v>0</v>
@@ -7244,22 +7253,22 @@
       <c r="E191" s="20">
         <v>1</v>
       </c>
-      <c r="F191" s="22">
+      <c r="F191" s="20">
         <v>1</v>
       </c>
       <c r="G191" s="3">
         <v>0</v>
       </c>
       <c r="H191" s="17" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" s="17" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B192" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C192" s="2">
         <v>0</v>
@@ -7277,15 +7286,15 @@
         <v>0</v>
       </c>
       <c r="H192" s="17" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" s="17" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B193" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C193" s="2">
         <v>0</v>
@@ -7303,15 +7312,15 @@
         <v>0</v>
       </c>
       <c r="H193" s="17" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" s="17" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B194" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C194" s="2">
         <v>0</v>
@@ -7329,15 +7338,15 @@
         <v>0</v>
       </c>
       <c r="H194" s="17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" s="17" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B195" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C195" s="2">
         <v>0</v>
@@ -7355,15 +7364,15 @@
         <v>0</v>
       </c>
       <c r="H195" s="17" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" s="17" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B196" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C196" s="2">
         <v>0</v>
@@ -7381,15 +7390,15 @@
         <v>0</v>
       </c>
       <c r="H196" s="17" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" s="17" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B197" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C197" s="2">
         <v>0</v>
@@ -7407,15 +7416,15 @@
         <v>0</v>
       </c>
       <c r="H197" s="17" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" s="17" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B198" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C198" s="2">
         <v>0</v>
@@ -7433,67 +7442,67 @@
         <v>0</v>
       </c>
       <c r="H198" s="17" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" s="17" t="s">
+        <v>475</v>
+      </c>
+      <c r="B199" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="C199" s="2">
+        <v>0</v>
+      </c>
+      <c r="D199" s="2">
+        <v>0</v>
+      </c>
+      <c r="E199" s="20">
+        <v>1</v>
+      </c>
+      <c r="F199" s="22">
+        <v>1</v>
+      </c>
+      <c r="G199" s="3">
+        <v>0</v>
+      </c>
+      <c r="H199" s="17" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A200" s="17" t="s">
         <v>476</v>
       </c>
-      <c r="B199" s="14" t="s">
+      <c r="B200" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="C199" s="2">
-        <v>0</v>
-      </c>
-      <c r="D199" s="2">
-        <v>0</v>
-      </c>
-      <c r="E199" s="20">
-        <v>1</v>
-      </c>
-      <c r="F199" s="22">
-        <v>1</v>
-      </c>
-      <c r="G199" s="3">
-        <v>0</v>
-      </c>
-      <c r="H199" s="17" t="s">
+      <c r="C200" s="2">
+        <v>0</v>
+      </c>
+      <c r="D200" s="2">
+        <v>0</v>
+      </c>
+      <c r="E200" s="20">
+        <v>1</v>
+      </c>
+      <c r="F200" s="22">
+        <v>1</v>
+      </c>
+      <c r="G200" s="3">
+        <v>0</v>
+      </c>
+      <c r="H200" s="17" t="s">
         <v>326</v>
-      </c>
-    </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A200" s="18" t="s">
-        <v>477</v>
-      </c>
-      <c r="B200" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="C200" s="2">
-        <v>0</v>
-      </c>
-      <c r="D200" s="2">
-        <v>0</v>
-      </c>
-      <c r="E200" s="20">
-        <v>1</v>
-      </c>
-      <c r="F200" s="22">
-        <v>1</v>
-      </c>
-      <c r="G200" s="3">
-        <v>0</v>
-      </c>
-      <c r="H200" s="18" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" s="18" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B201" s="16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C201" s="2">
         <v>0</v>
@@ -7511,15 +7520,15 @@
         <v>0</v>
       </c>
       <c r="H201" s="18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" s="18" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B202" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C202" s="2">
         <v>0</v>
@@ -7537,15 +7546,15 @@
         <v>0</v>
       </c>
       <c r="H202" s="18" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203" s="18" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B203" s="16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C203" s="2">
         <v>0</v>
@@ -7563,15 +7572,15 @@
         <v>0</v>
       </c>
       <c r="H203" s="18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A204" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B204" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C204" s="2">
         <v>0</v>
@@ -7589,15 +7598,15 @@
         <v>0</v>
       </c>
       <c r="H204" s="18" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205" s="18" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B205" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C205" s="2">
         <v>0</v>
@@ -7615,15 +7624,15 @@
         <v>0</v>
       </c>
       <c r="H205" s="18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B206" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C206" s="2">
         <v>0</v>
@@ -7641,32 +7650,58 @@
         <v>0</v>
       </c>
       <c r="H206" s="18" t="s">
-        <v>213</v>
+        <v>332</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" s="18" t="s">
+        <v>483</v>
+      </c>
+      <c r="B207" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="C207" s="2">
+        <v>0</v>
+      </c>
+      <c r="D207" s="2">
+        <v>0</v>
+      </c>
+      <c r="E207" s="20">
+        <v>1</v>
+      </c>
+      <c r="F207" s="22">
+        <v>1</v>
+      </c>
+      <c r="G207" s="3">
+        <v>0</v>
+      </c>
+      <c r="H207" s="18" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A208" s="18" t="s">
         <v>484</v>
       </c>
-      <c r="B207" s="16" t="s">
+      <c r="B208" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="C207" s="2">
-        <v>0</v>
-      </c>
-      <c r="D207" s="2">
-        <v>0</v>
-      </c>
-      <c r="E207" s="20">
-        <v>1</v>
-      </c>
-      <c r="F207" s="20">
-        <v>1</v>
-      </c>
-      <c r="G207" s="3">
-        <v>0</v>
-      </c>
-      <c r="H207" s="18" t="s">
+      <c r="C208" s="2">
+        <v>0</v>
+      </c>
+      <c r="D208" s="2">
+        <v>0</v>
+      </c>
+      <c r="E208" s="20">
+        <v>1</v>
+      </c>
+      <c r="F208" s="20">
+        <v>1</v>
+      </c>
+      <c r="G208" s="3">
+        <v>0</v>
+      </c>
+      <c r="H208" s="18" t="s">
         <v>212</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Kenya LS export: fix measurements and add lost to consultation
</commit_message>
<xml_diff>
--- a/inst/extdata/main_dict_kenya.xlsx
+++ b/inst/extdata/main_dict_kenya.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="615">
   <si>
     <t>old</t>
   </si>
@@ -1784,42 +1784,6 @@
     <t>rx_salbutamol_route</t>
   </si>
   <si>
-    <t>crfs-t07a-tt06a-d2_6</t>
-  </si>
-  <si>
-    <t>crfs-t07a-tt06a-d2_1</t>
-  </si>
-  <si>
-    <t>crfs-t07a-tt06a-d2_6b</t>
-  </si>
-  <si>
-    <t>crfs-t07a-tt06a-d2_1a</t>
-  </si>
-  <si>
-    <t>crfs-t07a-tt06a-d2_4</t>
-  </si>
-  <si>
-    <t>crfs-t07a-tt06a-d2_4a</t>
-  </si>
-  <si>
-    <t>crfs-t07a-tt06a-d2_5</t>
-  </si>
-  <si>
-    <t>crfs-t07a-tt06a-d2_5a</t>
-  </si>
-  <si>
-    <t>crfs-t07a-tt06a-d2_2</t>
-  </si>
-  <si>
-    <t>crfs-t07a-tt06a-d2_2b</t>
-  </si>
-  <si>
-    <t>crfs-t07a-tt06a-d2_3</t>
-  </si>
-  <si>
-    <t>crfs-t07a-tt06a-d2_3b</t>
-  </si>
-  <si>
     <t>crfs-t02b-location_name</t>
   </si>
   <si>
@@ -1860,6 +1824,51 @@
   </si>
   <si>
     <t>a4_a_10a</t>
+  </si>
+  <si>
+    <t>crfs-t06a-tt06a-d2_6</t>
+  </si>
+  <si>
+    <t>crfs-t06a-tt06a-d2_6b</t>
+  </si>
+  <si>
+    <t>crfs-t06a-tt06a-d2_1</t>
+  </si>
+  <si>
+    <t>crfs-t06a-tt06a-d2_1a</t>
+  </si>
+  <si>
+    <t>crfs-t06a-tt06a-d2_4</t>
+  </si>
+  <si>
+    <t>crfs-t06a-tt06a-d2_4a</t>
+  </si>
+  <si>
+    <t>crfs-t06a-tt06a-d2_5</t>
+  </si>
+  <si>
+    <t>crfs-t06a-tt06a-d2_5a</t>
+  </si>
+  <si>
+    <t>crfs-t06a-tt06a-d2_2</t>
+  </si>
+  <si>
+    <t>crfs-t06a-tt06a-d2_2b</t>
+  </si>
+  <si>
+    <t>crfs-t06a-tt06a-d2_3</t>
+  </si>
+  <si>
+    <t>crfs-t06a-tt06a-d2_3b</t>
+  </si>
+  <si>
+    <t>crfs-t09a1-exit_yn</t>
+  </si>
+  <si>
+    <t>lost_at_consultation_exit</t>
+  </si>
+  <si>
+    <t>exit_yn</t>
   </si>
 </sst>
 </file>
@@ -2280,10 +2289,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H208"/>
+  <dimension ref="A1:H209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="K127" sqref="K127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2429,10 +2438,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>601</v>
+        <v>589</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>601</v>
+        <v>589</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -2450,7 +2459,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>601</v>
+        <v>589</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -2796,7 +2805,7 @@
         <v>341</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>608</v>
+        <v>596</v>
       </c>
       <c r="C20" s="2">
         <v>1</v>
@@ -3573,10 +3582,10 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
-        <v>609</v>
+        <v>597</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>610</v>
+        <v>598</v>
       </c>
       <c r="C50" s="2">
         <v>0</v>
@@ -3594,7 +3603,7 @@
         <v>1</v>
       </c>
       <c r="H50" s="11" t="s">
-        <v>611</v>
+        <v>599</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -3885,7 +3894,7 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
-        <v>598</v>
+        <v>586</v>
       </c>
       <c r="B62" s="11" t="s">
         <v>502</v>
@@ -3911,10 +3920,10 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="11" t="s">
-        <v>599</v>
+        <v>587</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>600</v>
+        <v>588</v>
       </c>
       <c r="C63" s="2">
         <v>1</v>
@@ -5549,10 +5558,10 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" s="17" t="s">
-        <v>441</v>
-      </c>
-      <c r="B126" s="14" t="s">
-        <v>113</v>
+        <v>612</v>
+      </c>
+      <c r="B126" s="15" t="s">
+        <v>613</v>
       </c>
       <c r="C126" s="2">
         <v>0</v>
@@ -5563,22 +5572,22 @@
       <c r="E126" s="20">
         <v>1</v>
       </c>
-      <c r="F126" s="22">
+      <c r="F126" s="20">
         <v>1</v>
       </c>
       <c r="G126" s="3">
         <v>1</v>
       </c>
       <c r="H126" s="17" t="s">
-        <v>279</v>
+        <v>614</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" s="17" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B127" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C127" s="2">
         <v>0</v>
@@ -5593,18 +5602,18 @@
         <v>1</v>
       </c>
       <c r="G127" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H127" s="17" t="s">
-        <v>114</v>
+        <v>279</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" s="17" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B128" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C128" s="2">
         <v>0</v>
@@ -5622,15 +5631,15 @@
         <v>0</v>
       </c>
       <c r="H128" s="17" t="s">
-        <v>280</v>
+        <v>114</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" s="17" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B129" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C129" s="2">
         <v>0</v>
@@ -5648,15 +5657,15 @@
         <v>0</v>
       </c>
       <c r="H129" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" s="17" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B130" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C130" s="2">
         <v>0</v>
@@ -5674,15 +5683,15 @@
         <v>0</v>
       </c>
       <c r="H130" s="17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" s="17" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B131" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C131" s="2">
         <v>0</v>
@@ -5693,22 +5702,22 @@
       <c r="E131" s="20">
         <v>1</v>
       </c>
-      <c r="F131" s="20">
+      <c r="F131" s="22">
         <v>1</v>
       </c>
       <c r="G131" s="3">
         <v>0</v>
       </c>
       <c r="H131" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" s="17" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B132" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C132" s="2">
         <v>0</v>
@@ -5719,22 +5728,22 @@
       <c r="E132" s="20">
         <v>1</v>
       </c>
-      <c r="F132" s="22">
+      <c r="F132" s="20">
         <v>1</v>
       </c>
       <c r="G132" s="3">
         <v>0</v>
       </c>
       <c r="H132" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" s="17" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B133" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C133" s="2">
         <v>0</v>
@@ -5752,67 +5761,67 @@
         <v>0</v>
       </c>
       <c r="H133" s="17" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" s="17" t="s">
+        <v>448</v>
+      </c>
+      <c r="B134" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C134" s="2">
+        <v>0</v>
+      </c>
+      <c r="D134" s="2">
+        <v>0</v>
+      </c>
+      <c r="E134" s="20">
+        <v>1</v>
+      </c>
+      <c r="F134" s="22">
+        <v>1</v>
+      </c>
+      <c r="G134" s="3">
+        <v>0</v>
+      </c>
+      <c r="H134" s="17" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A135" s="17" t="s">
         <v>449</v>
       </c>
-      <c r="B134" s="14" t="s">
+      <c r="B135" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="C134" s="2">
-        <v>0</v>
-      </c>
-      <c r="D134" s="2">
-        <v>0</v>
-      </c>
-      <c r="E134" s="20">
-        <v>1</v>
-      </c>
-      <c r="F134" s="22">
-        <v>1</v>
-      </c>
-      <c r="G134" s="3">
-        <v>0</v>
-      </c>
-      <c r="H134" s="17" t="s">
+      <c r="C135" s="2">
+        <v>0</v>
+      </c>
+      <c r="D135" s="2">
+        <v>0</v>
+      </c>
+      <c r="E135" s="20">
+        <v>1</v>
+      </c>
+      <c r="F135" s="22">
+        <v>1</v>
+      </c>
+      <c r="G135" s="3">
+        <v>0</v>
+      </c>
+      <c r="H135" s="17" t="s">
         <v>286</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A135" s="18" t="s">
-        <v>574</v>
-      </c>
-      <c r="B135" s="16" t="s">
-        <v>580</v>
-      </c>
-      <c r="C135" s="2">
-        <v>0</v>
-      </c>
-      <c r="D135" s="2">
-        <v>0</v>
-      </c>
-      <c r="E135" s="20">
-        <v>1</v>
-      </c>
-      <c r="F135" s="20">
-        <v>1</v>
-      </c>
-      <c r="G135" s="3">
-        <v>0</v>
-      </c>
-      <c r="H135" s="18" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" s="18" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B136" s="16" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C136" s="2">
         <v>0</v>
@@ -5830,15 +5839,15 @@
         <v>0</v>
       </c>
       <c r="H136" s="18" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" s="18" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B137" s="16" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C137" s="2">
         <v>0</v>
@@ -5856,15 +5865,15 @@
         <v>0</v>
       </c>
       <c r="H137" s="18" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" s="18" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B138" s="16" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C138" s="2">
         <v>0</v>
@@ -5882,15 +5891,15 @@
         <v>0</v>
       </c>
       <c r="H138" s="18" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" s="18" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B139" s="16" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C139" s="2">
         <v>0</v>
@@ -5908,67 +5917,67 @@
         <v>0</v>
       </c>
       <c r="H139" s="18" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" s="18" t="s">
+        <v>578</v>
+      </c>
+      <c r="B140" s="16" t="s">
+        <v>584</v>
+      </c>
+      <c r="C140" s="2">
+        <v>0</v>
+      </c>
+      <c r="D140" s="2">
+        <v>0</v>
+      </c>
+      <c r="E140" s="20">
+        <v>1</v>
+      </c>
+      <c r="F140" s="20">
+        <v>1</v>
+      </c>
+      <c r="G140" s="3">
+        <v>0</v>
+      </c>
+      <c r="H140" s="18" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A141" s="18" t="s">
         <v>579</v>
       </c>
-      <c r="B140" s="16" t="s">
+      <c r="B141" s="16" t="s">
         <v>585</v>
       </c>
-      <c r="C140" s="2">
-        <v>0</v>
-      </c>
-      <c r="D140" s="2">
-        <v>0</v>
-      </c>
-      <c r="E140" s="20">
-        <v>1</v>
-      </c>
-      <c r="F140" s="20">
-        <v>1</v>
-      </c>
-      <c r="G140" s="3">
-        <v>0</v>
-      </c>
-      <c r="H140" s="18" t="s">
+      <c r="C141" s="2">
+        <v>0</v>
+      </c>
+      <c r="D141" s="2">
+        <v>0</v>
+      </c>
+      <c r="E141" s="20">
+        <v>1</v>
+      </c>
+      <c r="F141" s="20">
+        <v>1</v>
+      </c>
+      <c r="G141" s="3">
+        <v>0</v>
+      </c>
+      <c r="H141" s="18" t="s">
         <v>555</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A141" s="17" t="s">
-        <v>450</v>
-      </c>
-      <c r="B141" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="C141" s="2">
-        <v>0</v>
-      </c>
-      <c r="D141" s="2">
-        <v>0</v>
-      </c>
-      <c r="E141" s="20">
-        <v>1</v>
-      </c>
-      <c r="F141" s="22">
-        <v>1</v>
-      </c>
-      <c r="G141" s="3">
-        <v>0</v>
-      </c>
-      <c r="H141" s="17" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" s="17" t="s">
-        <v>556</v>
-      </c>
-      <c r="B142" s="23" t="s">
-        <v>532</v>
+        <v>450</v>
+      </c>
+      <c r="B142" s="14" t="s">
+        <v>122</v>
       </c>
       <c r="C142" s="2">
         <v>0</v>
@@ -5976,7 +5985,7 @@
       <c r="D142" s="2">
         <v>0</v>
       </c>
-      <c r="E142" s="4">
+      <c r="E142" s="20">
         <v>1</v>
       </c>
       <c r="F142" s="22">
@@ -5986,15 +5995,15 @@
         <v>0</v>
       </c>
       <c r="H142" s="17" t="s">
-        <v>514</v>
+        <v>287</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" s="17" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B143" s="23" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C143" s="2">
         <v>0</v>
@@ -6012,15 +6021,15 @@
         <v>0</v>
       </c>
       <c r="H143" s="17" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" s="17" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B144" s="23" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="C144" s="2">
         <v>0</v>
@@ -6038,15 +6047,15 @@
         <v>0</v>
       </c>
       <c r="H144" s="17" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" s="17" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B145" s="23" t="s">
-        <v>534</v>
+        <v>539</v>
       </c>
       <c r="C145" s="2">
         <v>0</v>
@@ -6064,15 +6073,15 @@
         <v>0</v>
       </c>
       <c r="H145" s="17" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" s="17" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B146" s="23" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="C146" s="2">
         <v>0</v>
@@ -6090,15 +6099,15 @@
         <v>0</v>
       </c>
       <c r="H146" s="17" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" s="17" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B147" s="23" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C147" s="2">
         <v>0</v>
@@ -6116,15 +6125,15 @@
         <v>0</v>
       </c>
       <c r="H147" s="17" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" s="17" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B148" s="23" t="s">
-        <v>535</v>
+        <v>541</v>
       </c>
       <c r="C148" s="2">
         <v>0</v>
@@ -6142,15 +6151,15 @@
         <v>0</v>
       </c>
       <c r="H148" s="17" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" s="17" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B149" s="23" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="C149" s="2">
         <v>0</v>
@@ -6168,15 +6177,15 @@
         <v>0</v>
       </c>
       <c r="H149" s="17" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" s="17" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B150" s="23" t="s">
-        <v>536</v>
+        <v>542</v>
       </c>
       <c r="C150" s="2">
         <v>0</v>
@@ -6194,15 +6203,15 @@
         <v>0</v>
       </c>
       <c r="H150" s="17" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" s="17" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B151" s="23" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="C151" s="2">
         <v>0</v>
@@ -6220,15 +6229,15 @@
         <v>0</v>
       </c>
       <c r="H151" s="17" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" s="17" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B152" s="23" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C152" s="2">
         <v>0</v>
@@ -6246,15 +6255,15 @@
         <v>0</v>
       </c>
       <c r="H152" s="17" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" s="17" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B153" s="23" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C153" s="2">
         <v>0</v>
@@ -6272,15 +6281,15 @@
         <v>0</v>
       </c>
       <c r="H153" s="17" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" s="17" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B154" s="23" t="s">
-        <v>537</v>
+        <v>545</v>
       </c>
       <c r="C154" s="2">
         <v>0</v>
@@ -6298,15 +6307,15 @@
         <v>0</v>
       </c>
       <c r="H154" s="17" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" s="17" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B155" s="23" t="s">
-        <v>546</v>
+        <v>537</v>
       </c>
       <c r="C155" s="2">
         <v>0</v>
@@ -6324,15 +6333,15 @@
         <v>0</v>
       </c>
       <c r="H155" s="17" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" s="17" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B156" s="23" t="s">
-        <v>538</v>
+        <v>546</v>
       </c>
       <c r="C156" s="2">
         <v>0</v>
@@ -6350,15 +6359,15 @@
         <v>0</v>
       </c>
       <c r="H156" s="17" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" s="17" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B157" s="23" t="s">
-        <v>547</v>
+        <v>538</v>
       </c>
       <c r="C157" s="2">
         <v>0</v>
@@ -6376,15 +6385,15 @@
         <v>0</v>
       </c>
       <c r="H157" s="17" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" s="17" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B158" s="23" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C158" s="2">
         <v>0</v>
@@ -6402,15 +6411,15 @@
         <v>0</v>
       </c>
       <c r="H158" s="17" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" s="17" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B159" s="23" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="C159" s="2">
         <v>0</v>
@@ -6428,15 +6437,15 @@
         <v>0</v>
       </c>
       <c r="H159" s="17" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" s="17" t="s">
-        <v>451</v>
-      </c>
-      <c r="B160" s="14" t="s">
-        <v>123</v>
+        <v>573</v>
+      </c>
+      <c r="B160" s="23" t="s">
+        <v>548</v>
       </c>
       <c r="C160" s="2">
         <v>0</v>
@@ -6444,7 +6453,7 @@
       <c r="D160" s="2">
         <v>0</v>
       </c>
-      <c r="E160" s="20">
+      <c r="E160" s="4">
         <v>1</v>
       </c>
       <c r="F160" s="22">
@@ -6454,15 +6463,15 @@
         <v>0</v>
       </c>
       <c r="H160" s="17" t="s">
-        <v>288</v>
+        <v>531</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" s="17" t="s">
-        <v>416</v>
+        <v>451</v>
       </c>
       <c r="B161" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C161" s="2">
         <v>0</v>
@@ -6480,15 +6489,15 @@
         <v>0</v>
       </c>
       <c r="H161" s="17" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" s="17" t="s">
-        <v>452</v>
+        <v>416</v>
       </c>
       <c r="B162" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C162" s="2">
         <v>0</v>
@@ -6503,18 +6512,18 @@
         <v>1</v>
       </c>
       <c r="G162" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H162" s="17" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" s="17" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B163" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C163" s="2">
         <v>0</v>
@@ -6532,15 +6541,15 @@
         <v>1</v>
       </c>
       <c r="H163" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" s="17" t="s">
-        <v>602</v>
+        <v>453</v>
       </c>
       <c r="B164" s="14" t="s">
-        <v>603</v>
+        <v>126</v>
       </c>
       <c r="C164" s="2">
         <v>0</v>
@@ -6558,15 +6567,15 @@
         <v>1</v>
       </c>
       <c r="H164" s="17" t="s">
-        <v>604</v>
+        <v>291</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" s="17" t="s">
-        <v>605</v>
+        <v>590</v>
       </c>
       <c r="B165" s="14" t="s">
-        <v>606</v>
+        <v>591</v>
       </c>
       <c r="C165" s="2">
         <v>0</v>
@@ -6584,15 +6593,15 @@
         <v>1</v>
       </c>
       <c r="H165" s="17" t="s">
-        <v>607</v>
+        <v>592</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" s="17" t="s">
-        <v>454</v>
-      </c>
-      <c r="B166" s="15" t="s">
-        <v>127</v>
+        <v>593</v>
+      </c>
+      <c r="B166" s="14" t="s">
+        <v>594</v>
       </c>
       <c r="C166" s="2">
         <v>0</v>
@@ -6607,18 +6616,18 @@
         <v>1</v>
       </c>
       <c r="G166" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H166" s="17" t="s">
-        <v>292</v>
+        <v>595</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" s="17" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B167" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C167" s="2">
         <v>0</v>
@@ -6636,15 +6645,15 @@
         <v>0</v>
       </c>
       <c r="H167" s="17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" s="17" t="s">
-        <v>456</v>
-      </c>
-      <c r="B168" s="14" t="s">
-        <v>129</v>
+        <v>455</v>
+      </c>
+      <c r="B168" s="15" t="s">
+        <v>128</v>
       </c>
       <c r="C168" s="2">
         <v>0</v>
@@ -6662,15 +6671,15 @@
         <v>0</v>
       </c>
       <c r="H168" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" s="17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B169" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C169" s="2">
         <v>0</v>
@@ -6681,22 +6690,22 @@
       <c r="E169" s="20">
         <v>1</v>
       </c>
-      <c r="F169" s="20">
+      <c r="F169" s="22">
         <v>1</v>
       </c>
       <c r="G169" s="3">
         <v>0</v>
       </c>
       <c r="H169" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" s="17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B170" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C170" s="2">
         <v>0</v>
@@ -6707,22 +6716,22 @@
       <c r="E170" s="20">
         <v>1</v>
       </c>
-      <c r="F170" s="22">
+      <c r="F170" s="20">
         <v>1</v>
       </c>
       <c r="G170" s="3">
         <v>0</v>
       </c>
       <c r="H170" s="17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" s="17" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B171" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C171" s="2">
         <v>0</v>
@@ -6740,15 +6749,15 @@
         <v>0</v>
       </c>
       <c r="H171" s="17" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" s="17" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B172" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C172" s="2">
         <v>0</v>
@@ -6763,18 +6772,18 @@
         <v>1</v>
       </c>
       <c r="G172" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H172" s="17" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" s="17" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B173" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C173" s="2">
         <v>0</v>
@@ -6792,15 +6801,15 @@
         <v>1</v>
       </c>
       <c r="H173" s="17" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" s="17" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B174" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C174" s="2">
         <v>0</v>
@@ -6815,18 +6824,18 @@
         <v>1</v>
       </c>
       <c r="G174" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H174" s="17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" s="17" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B175" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C175" s="2">
         <v>0</v>
@@ -6844,15 +6853,15 @@
         <v>0</v>
       </c>
       <c r="H175" s="17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" s="17" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B176" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C176" s="2">
         <v>0</v>
@@ -6870,15 +6879,15 @@
         <v>0</v>
       </c>
       <c r="H176" s="17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" s="17" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B177" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C177" s="2">
         <v>0</v>
@@ -6896,15 +6905,15 @@
         <v>0</v>
       </c>
       <c r="H177" s="17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" s="17" t="s">
-        <v>586</v>
+        <v>465</v>
       </c>
       <c r="B178" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C178" s="2">
         <v>0</v>
@@ -6922,15 +6931,15 @@
         <v>0</v>
       </c>
       <c r="H178" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" s="17" t="s">
-        <v>588</v>
+        <v>600</v>
       </c>
       <c r="B179" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C179" s="2">
         <v>0</v>
@@ -6948,15 +6957,15 @@
         <v>0</v>
       </c>
       <c r="H179" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" s="17" t="s">
-        <v>587</v>
+        <v>601</v>
       </c>
       <c r="B180" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C180" s="2">
         <v>0</v>
@@ -6974,15 +6983,15 @@
         <v>0</v>
       </c>
       <c r="H180" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" s="17" t="s">
-        <v>589</v>
+        <v>602</v>
       </c>
       <c r="B181" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C181" s="2">
         <v>0</v>
@@ -7000,15 +7009,15 @@
         <v>0</v>
       </c>
       <c r="H181" s="17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" s="17" t="s">
-        <v>590</v>
+        <v>603</v>
       </c>
       <c r="B182" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C182" s="2">
         <v>0</v>
@@ -7026,15 +7035,15 @@
         <v>0</v>
       </c>
       <c r="H182" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" s="17" t="s">
-        <v>591</v>
+        <v>604</v>
       </c>
       <c r="B183" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C183" s="2">
         <v>0</v>
@@ -7052,15 +7061,15 @@
         <v>0</v>
       </c>
       <c r="H183" s="17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" s="17" t="s">
-        <v>592</v>
+        <v>605</v>
       </c>
       <c r="B184" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C184" s="2">
         <v>0</v>
@@ -7078,15 +7087,15 @@
         <v>0</v>
       </c>
       <c r="H184" s="17" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" s="17" t="s">
-        <v>593</v>
+        <v>606</v>
       </c>
       <c r="B185" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C185" s="2">
         <v>0</v>
@@ -7104,15 +7113,15 @@
         <v>0</v>
       </c>
       <c r="H185" s="17" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" s="17" t="s">
-        <v>594</v>
+        <v>607</v>
       </c>
       <c r="B186" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C186" s="2">
         <v>0</v>
@@ -7130,15 +7139,15 @@
         <v>0</v>
       </c>
       <c r="H186" s="17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" s="17" t="s">
-        <v>595</v>
+        <v>608</v>
       </c>
       <c r="B187" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C187" s="2">
         <v>0</v>
@@ -7156,15 +7165,15 @@
         <v>0</v>
       </c>
       <c r="H187" s="17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" s="17" t="s">
-        <v>596</v>
+        <v>609</v>
       </c>
       <c r="B188" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C188" s="2">
         <v>0</v>
@@ -7182,15 +7191,15 @@
         <v>0</v>
       </c>
       <c r="H188" s="17" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" s="17" t="s">
-        <v>597</v>
+        <v>610</v>
       </c>
       <c r="B189" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C189" s="2">
         <v>0</v>
@@ -7208,15 +7217,15 @@
         <v>0</v>
       </c>
       <c r="H189" s="17" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" s="17" t="s">
-        <v>466</v>
+        <v>611</v>
       </c>
       <c r="B190" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C190" s="2">
         <v>0</v>
@@ -7234,15 +7243,15 @@
         <v>0</v>
       </c>
       <c r="H190" s="17" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" s="17" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B191" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C191" s="2">
         <v>0</v>
@@ -7253,22 +7262,22 @@
       <c r="E191" s="20">
         <v>1</v>
       </c>
-      <c r="F191" s="20">
+      <c r="F191" s="22">
         <v>1</v>
       </c>
       <c r="G191" s="3">
         <v>0</v>
       </c>
       <c r="H191" s="17" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B192" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C192" s="2">
         <v>0</v>
@@ -7279,22 +7288,22 @@
       <c r="E192" s="20">
         <v>1</v>
       </c>
-      <c r="F192" s="22">
+      <c r="F192" s="20">
         <v>1</v>
       </c>
       <c r="G192" s="3">
         <v>0</v>
       </c>
       <c r="H192" s="17" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" s="17" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B193" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C193" s="2">
         <v>0</v>
@@ -7312,15 +7321,15 @@
         <v>0</v>
       </c>
       <c r="H193" s="17" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" s="17" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B194" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C194" s="2">
         <v>0</v>
@@ -7338,15 +7347,15 @@
         <v>0</v>
       </c>
       <c r="H194" s="17" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" s="17" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B195" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C195" s="2">
         <v>0</v>
@@ -7364,15 +7373,15 @@
         <v>0</v>
       </c>
       <c r="H195" s="17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" s="17" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B196" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C196" s="2">
         <v>0</v>
@@ -7390,15 +7399,15 @@
         <v>0</v>
       </c>
       <c r="H196" s="17" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" s="17" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B197" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C197" s="2">
         <v>0</v>
@@ -7416,15 +7425,15 @@
         <v>0</v>
       </c>
       <c r="H197" s="17" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" s="17" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B198" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C198" s="2">
         <v>0</v>
@@ -7442,15 +7451,15 @@
         <v>0</v>
       </c>
       <c r="H198" s="17" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" s="17" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B199" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C199" s="2">
         <v>0</v>
@@ -7468,67 +7477,67 @@
         <v>0</v>
       </c>
       <c r="H199" s="17" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" s="17" t="s">
+        <v>475</v>
+      </c>
+      <c r="B200" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="C200" s="2">
+        <v>0</v>
+      </c>
+      <c r="D200" s="2">
+        <v>0</v>
+      </c>
+      <c r="E200" s="20">
+        <v>1</v>
+      </c>
+      <c r="F200" s="22">
+        <v>1</v>
+      </c>
+      <c r="G200" s="3">
+        <v>0</v>
+      </c>
+      <c r="H200" s="17" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A201" s="17" t="s">
         <v>476</v>
       </c>
-      <c r="B200" s="14" t="s">
+      <c r="B201" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="C200" s="2">
-        <v>0</v>
-      </c>
-      <c r="D200" s="2">
-        <v>0</v>
-      </c>
-      <c r="E200" s="20">
-        <v>1</v>
-      </c>
-      <c r="F200" s="22">
-        <v>1</v>
-      </c>
-      <c r="G200" s="3">
-        <v>0</v>
-      </c>
-      <c r="H200" s="17" t="s">
+      <c r="C201" s="2">
+        <v>0</v>
+      </c>
+      <c r="D201" s="2">
+        <v>0</v>
+      </c>
+      <c r="E201" s="20">
+        <v>1</v>
+      </c>
+      <c r="F201" s="22">
+        <v>1</v>
+      </c>
+      <c r="G201" s="3">
+        <v>0</v>
+      </c>
+      <c r="H201" s="17" t="s">
         <v>326</v>
-      </c>
-    </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A201" s="18" t="s">
-        <v>477</v>
-      </c>
-      <c r="B201" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="C201" s="2">
-        <v>0</v>
-      </c>
-      <c r="D201" s="2">
-        <v>0</v>
-      </c>
-      <c r="E201" s="20">
-        <v>1</v>
-      </c>
-      <c r="F201" s="22">
-        <v>1</v>
-      </c>
-      <c r="G201" s="3">
-        <v>0</v>
-      </c>
-      <c r="H201" s="18" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" s="18" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B202" s="16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C202" s="2">
         <v>0</v>
@@ -7546,15 +7555,15 @@
         <v>0</v>
       </c>
       <c r="H202" s="18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203" s="18" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B203" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C203" s="2">
         <v>0</v>
@@ -7572,15 +7581,15 @@
         <v>0</v>
       </c>
       <c r="H203" s="18" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A204" s="18" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B204" s="16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C204" s="2">
         <v>0</v>
@@ -7598,15 +7607,15 @@
         <v>0</v>
       </c>
       <c r="H204" s="18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B205" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C205" s="2">
         <v>0</v>
@@ -7624,15 +7633,15 @@
         <v>0</v>
       </c>
       <c r="H205" s="18" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206" s="18" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B206" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C206" s="2">
         <v>0</v>
@@ -7650,15 +7659,15 @@
         <v>0</v>
       </c>
       <c r="H206" s="18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B207" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C207" s="2">
         <v>0</v>
@@ -7676,32 +7685,58 @@
         <v>0</v>
       </c>
       <c r="H207" s="18" t="s">
-        <v>213</v>
+        <v>332</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208" s="18" t="s">
+        <v>483</v>
+      </c>
+      <c r="B208" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="C208" s="2">
+        <v>0</v>
+      </c>
+      <c r="D208" s="2">
+        <v>0</v>
+      </c>
+      <c r="E208" s="20">
+        <v>1</v>
+      </c>
+      <c r="F208" s="22">
+        <v>1</v>
+      </c>
+      <c r="G208" s="3">
+        <v>0</v>
+      </c>
+      <c r="H208" s="18" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A209" s="18" t="s">
         <v>484</v>
       </c>
-      <c r="B208" s="16" t="s">
+      <c r="B209" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="C208" s="2">
-        <v>0</v>
-      </c>
-      <c r="D208" s="2">
-        <v>0</v>
-      </c>
-      <c r="E208" s="20">
-        <v>1</v>
-      </c>
-      <c r="F208" s="20">
-        <v>1</v>
-      </c>
-      <c r="G208" s="3">
-        <v>0</v>
-      </c>
-      <c r="H208" s="18" t="s">
+      <c r="C209" s="2">
+        <v>0</v>
+      </c>
+      <c r="D209" s="2">
+        <v>0</v>
+      </c>
+      <c r="E209" s="20">
+        <v>1</v>
+      </c>
+      <c r="F209" s="20">
+        <v>1</v>
+      </c>
+      <c r="G209" s="3">
+        <v>0</v>
+      </c>
+      <c r="H209" s="18" t="s">
         <v>212</v>
       </c>
     </row>

</xml_diff>